<commit_message>
add boons, daedalus augments. Fix sectionTitle on updateSectionCompletion
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10606"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://rockyviewschools-my.sharepoint.com/personal/jguigue_rockyview_ab_ca/Documents/Desktop/HTML/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHubChelsea\HadesCompletion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="232" documentId="8_{156EE6A4-FC9D-9F45-85FA-4B7BBAB08DBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ACB7E3E6-2C71-CA4C-9877-E6E3E5EF42AC}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C81CC89C-F563-4A6F-8F9A-16E037607B82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14600" yWindow="0" windowWidth="14200" windowHeight="18000" xr2:uid="{E79D6183-D772-F644-AE89-4CAD504C8F4D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E79D6183-D772-F644-AE89-4CAD504C8F4D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="596" uniqueCount="558">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="865" uniqueCount="818">
   <si>
     <t>Fated List of Minor Prophecies</t>
   </si>
@@ -1710,13 +1710,793 @@
   </si>
   <si>
     <t>Styx Complete</t>
+  </si>
+  <si>
+    <t>Boons-Aphrodite</t>
+  </si>
+  <si>
+    <t>Num Checkboxes</t>
+  </si>
+  <si>
+    <t>Boons-Ares</t>
+  </si>
+  <si>
+    <t>Boons-Artemis</t>
+  </si>
+  <si>
+    <t>Boons-Athena</t>
+  </si>
+  <si>
+    <t>Boons-Demeter</t>
+  </si>
+  <si>
+    <t>Boons-Dionysus</t>
+  </si>
+  <si>
+    <t>Boons-Hermes</t>
+  </si>
+  <si>
+    <t>Boons-Poseidon</t>
+  </si>
+  <si>
+    <t>Boons-Zeus</t>
+  </si>
+  <si>
+    <t>Boons-Chaos</t>
+  </si>
+  <si>
+    <t>Duo-Boons</t>
+  </si>
+  <si>
+    <t>Aphrodite's Aid</t>
+  </si>
+  <si>
+    <t>Ares's Aid</t>
+  </si>
+  <si>
+    <t>Atremis' Aid</t>
+  </si>
+  <si>
+    <t>Athena's Aid</t>
+  </si>
+  <si>
+    <t>Arctic Blast</t>
+  </si>
+  <si>
+    <t>After Party</t>
+  </si>
+  <si>
+    <t>Bad News</t>
+  </si>
+  <si>
+    <t>Boiling Point</t>
+  </si>
+  <si>
+    <t>Billowing Strength</t>
+  </si>
+  <si>
+    <t>Abyssal Favor</t>
+  </si>
+  <si>
+    <t>Curse of Longing (Aphrodite &amp; Ares)</t>
+  </si>
+  <si>
+    <t>Blown Kiss</t>
+  </si>
+  <si>
+    <t>Battle Rage</t>
+  </si>
+  <si>
+    <t>Clean Kill</t>
+  </si>
+  <si>
+    <t>Blinding Flash</t>
+  </si>
+  <si>
+    <t>Crystal Beam</t>
+  </si>
+  <si>
+    <t>Bad Influence</t>
+  </si>
+  <si>
+    <t>Flurry Cast</t>
+  </si>
+  <si>
+    <t>Breaking Wave</t>
+  </si>
+  <si>
+    <t>Clouded Judgement</t>
+  </si>
+  <si>
+    <t>Abyssal Flourish</t>
+  </si>
+  <si>
+    <t>Heart Rend (Aphrodite &amp; Artemis)</t>
+  </si>
+  <si>
+    <t>Broken Resolve</t>
+  </si>
+  <si>
+    <t>Black Metal</t>
+  </si>
+  <si>
+    <t>Deadly Flourish</t>
+  </si>
+  <si>
+    <t>Brilliant Riposte</t>
+  </si>
+  <si>
+    <t>Demeter's Aid</t>
+  </si>
+  <si>
+    <t>Black Out</t>
+  </si>
+  <si>
+    <t>Greater Evasion</t>
+  </si>
+  <si>
+    <t>Flood Shot</t>
+  </si>
+  <si>
+    <t>Double Strike</t>
+  </si>
+  <si>
+    <t>Abyssal Strike</t>
+  </si>
+  <si>
+    <t>Parting Shot (Aphrodite &amp; Athena)</t>
+  </si>
+  <si>
+    <t>Crush Shot</t>
+  </si>
+  <si>
+    <t>Blade Dash</t>
+  </si>
+  <si>
+    <t>Deadly Strike</t>
+  </si>
+  <si>
+    <t>Bronze Skin</t>
+  </si>
+  <si>
+    <t>Frost Flourish</t>
+  </si>
+  <si>
+    <t>Dionysus' Aid</t>
+  </si>
+  <si>
+    <t>Greater Haste</t>
+  </si>
+  <si>
+    <t>Hydraulic Might</t>
+  </si>
+  <si>
+    <t>Electric Shot</t>
+  </si>
+  <si>
+    <t>Addled Grasp</t>
+  </si>
+  <si>
+    <t>Cold Embrace (Aphrodite &amp; Demeter)</t>
+  </si>
+  <si>
+    <t>Different League</t>
+  </si>
+  <si>
+    <t>Blood Frenzy</t>
+  </si>
+  <si>
+    <t>Exit Wounds</t>
+  </si>
+  <si>
+    <t>Divine Dash</t>
+  </si>
+  <si>
+    <t>Frost Strike</t>
+  </si>
+  <si>
+    <t>Drunken Dash</t>
+  </si>
+  <si>
+    <t>Greater Recall</t>
+  </si>
+  <si>
+    <t>Ocean's Bounty</t>
+  </si>
+  <si>
+    <t>Heaven's Vengeance</t>
+  </si>
+  <si>
+    <t>Caustic Ambush</t>
+  </si>
+  <si>
+    <t>Low Tolerance (Aphrodite &amp; Dionysus)</t>
+  </si>
+  <si>
+    <t>Dying Lament</t>
+  </si>
+  <si>
+    <t>Curse of Agony</t>
+  </si>
+  <si>
+    <t>Fully Loaded</t>
+  </si>
+  <si>
+    <t>Divine Flourish</t>
+  </si>
+  <si>
+    <t>Frozen Touch</t>
+  </si>
+  <si>
+    <t>Drunken Flourish</t>
+  </si>
+  <si>
+    <t>Greatest Reflex</t>
+  </si>
+  <si>
+    <t>Poseidon's Aid</t>
+  </si>
+  <si>
+    <t>High Voltage</t>
+  </si>
+  <si>
+    <t>Enshrouded Eclipse</t>
+  </si>
+  <si>
+    <t>Sweet Nectar (Aphrodite &amp; Poseidon)</t>
+  </si>
+  <si>
+    <t>Empty Inside</t>
+  </si>
+  <si>
+    <t>Curse of Pain</t>
+  </si>
+  <si>
+    <t>Hide Breaker</t>
+  </si>
+  <si>
+    <t>Divine Protection</t>
+  </si>
+  <si>
+    <t>Glacial Glare</t>
+  </si>
+  <si>
+    <t>Drunken Strike</t>
+  </si>
+  <si>
+    <t>Hyper Sprint</t>
+  </si>
+  <si>
+    <t>Razor Shoals</t>
+  </si>
+  <si>
+    <t>Lightning Reflexes</t>
+  </si>
+  <si>
+    <t>Enshrouded Favor</t>
+  </si>
+  <si>
+    <t>Smoldering Air (Aphrodite &amp; Zeus)</t>
+  </si>
+  <si>
+    <t>Heartbreak Flourish</t>
+  </si>
+  <si>
+    <t>Curse of Vengeance</t>
+  </si>
+  <si>
+    <t>Hunter Dash</t>
+  </si>
+  <si>
+    <t>Divine Strike</t>
+  </si>
+  <si>
+    <t>Killing Freeze</t>
+  </si>
+  <si>
+    <t>High Tolerance</t>
+  </si>
+  <si>
+    <t>Quick Favor</t>
+  </si>
+  <si>
+    <t>Rip Current</t>
+  </si>
+  <si>
+    <t>Lightning Strike</t>
+  </si>
+  <si>
+    <t>Enshrouded Grasp</t>
+  </si>
+  <si>
+    <t>Hunting Blades (Ares &amp; Artemis)</t>
+  </si>
+  <si>
+    <t>Heartbreak Strike</t>
+  </si>
+  <si>
+    <t>Dire Misfortune</t>
+  </si>
+  <si>
+    <t>Hunter Instinct</t>
+  </si>
+  <si>
+    <t>Holy Shield</t>
+  </si>
+  <si>
+    <t>Mistral Dash</t>
+  </si>
+  <si>
+    <t>Numbing Sensation</t>
+  </si>
+  <si>
+    <t>Quick Recovery</t>
+  </si>
+  <si>
+    <t>Second Wave</t>
+  </si>
+  <si>
+    <t>Splitting Bolt</t>
+  </si>
+  <si>
+    <t>Flayed Affluence</t>
+  </si>
+  <si>
+    <t>Merciful End (Ares &amp; Athena)</t>
+  </si>
+  <si>
+    <t>Life Affirmation</t>
+  </si>
+  <si>
+    <t>Englufing Vortex</t>
+  </si>
+  <si>
+    <t>Hunter's Mark</t>
+  </si>
+  <si>
+    <t>Phalanx Shot</t>
+  </si>
+  <si>
+    <t>Ravenous Will</t>
+  </si>
+  <si>
+    <t>Peer Pressure</t>
+  </si>
+  <si>
+    <t>Quick Reload</t>
+  </si>
+  <si>
+    <t>Tempest Flourish</t>
+  </si>
+  <si>
+    <t>Static Discharge</t>
+  </si>
+  <si>
+    <t>Halting Flourish</t>
+  </si>
+  <si>
+    <t>Freezing Vortex (Ares &amp; Demeter)</t>
+  </si>
+  <si>
+    <t>Passion Dash</t>
+  </si>
+  <si>
+    <t>Impending Doom</t>
+  </si>
+  <si>
+    <t>Pressure Points</t>
+  </si>
+  <si>
+    <t>Proud Breaing</t>
+  </si>
+  <si>
+    <t>Snow Burst</t>
+  </si>
+  <si>
+    <t>Positive Outlook</t>
+  </si>
+  <si>
+    <t>Rush Delivery</t>
+  </si>
+  <si>
+    <t>Tempest Strike</t>
+  </si>
+  <si>
+    <t>Storm Lightning</t>
+  </si>
+  <si>
+    <t>Maimed Soul</t>
+  </si>
+  <si>
+    <t>Curse of Nausea (Ares &amp; Dionysus)</t>
+  </si>
+  <si>
+    <t>Sweet Surrender</t>
+  </si>
+  <si>
+    <t>Slicing Shot</t>
+  </si>
+  <si>
+    <t>Support Fire</t>
+  </si>
+  <si>
+    <t>Sure Footing</t>
+  </si>
+  <si>
+    <t>Winter Harvest</t>
+  </si>
+  <si>
+    <t>Premium Vintage</t>
+  </si>
+  <si>
+    <t>Second Wind</t>
+  </si>
+  <si>
+    <t>Tidal Dash</t>
+  </si>
+  <si>
+    <t>Thunder Dash</t>
+  </si>
+  <si>
+    <t>Maimed Strike</t>
+  </si>
+  <si>
+    <t>Curse of Drowning (Ares &amp; Poseidon)</t>
+  </si>
+  <si>
+    <t>Unhealthy Fixation</t>
+  </si>
+  <si>
+    <t>Urge to Kill</t>
+  </si>
+  <si>
+    <t>True Shot</t>
+  </si>
+  <si>
+    <t>Strong Drink</t>
+  </si>
+  <si>
+    <t>Side Hustle</t>
+  </si>
+  <si>
+    <t>Typhoon's Fury</t>
+  </si>
+  <si>
+    <t>Thunder Flourish</t>
+  </si>
+  <si>
+    <t>Named Ambush</t>
+  </si>
+  <si>
+    <t>Vengeful Mood (Ares &amp; Zeus)</t>
+  </si>
+  <si>
+    <t>Wave of Despair</t>
+  </si>
+  <si>
+    <t>Vicious Cycle</t>
+  </si>
+  <si>
+    <t>Trippy Shot</t>
+  </si>
+  <si>
+    <t>Swift Flourish</t>
+  </si>
+  <si>
+    <t>Wave Pounding</t>
+  </si>
+  <si>
+    <t>Zeus' Aid</t>
+  </si>
+  <si>
+    <t>Pauper's Soul</t>
+  </si>
+  <si>
+    <t>Deadly Reversal (Artemis &amp; Athena)</t>
+  </si>
+  <si>
+    <t>Swift Strike</t>
+  </si>
+  <si>
+    <t>Roiling Eclipse</t>
+  </si>
+  <si>
+    <t>Crystal Clarity (Artemis &amp; Demeter)</t>
+  </si>
+  <si>
+    <t>Roiling Flourish</t>
+  </si>
+  <si>
+    <t>Splitting Headache (Artemis &amp; Dionysus)</t>
+  </si>
+  <si>
+    <t>Slippery Ambush</t>
+  </si>
+  <si>
+    <t>Mirage Shot (Artemis &amp; Poseidon)</t>
+  </si>
+  <si>
+    <t>Slippery Eclipse</t>
+  </si>
+  <si>
+    <t>Lightning Rod (Artemis &amp; Zeus)</t>
+  </si>
+  <si>
+    <t>Slippery Flourish</t>
+  </si>
+  <si>
+    <t>Stubborn Roots (Athena &amp; Demeter)</t>
+  </si>
+  <si>
+    <t>Slippery Shot</t>
+  </si>
+  <si>
+    <t>Calculated Risk (Athena &amp; Dionysus)</t>
+  </si>
+  <si>
+    <t>Unshakable Mettle (Athena &amp; Poseidon)</t>
+  </si>
+  <si>
+    <t>Lightning Phalanx (Athena &amp; Zeus)</t>
+  </si>
+  <si>
+    <t>Ice Wine (Demeter &amp; Dionysus)</t>
+  </si>
+  <si>
+    <t>Blizzard Shot (Demeter &amp; Poseidon)</t>
+  </si>
+  <si>
+    <t>Cold Fusion (Demeter &amp; Zeus)</t>
+  </si>
+  <si>
+    <t>Exclusive Access (Dionysus &amp; Poseidon)</t>
+  </si>
+  <si>
+    <t>Scintillating Feast (Dionysus &amp; Zeus)</t>
+  </si>
+  <si>
+    <t>Sea Storm (Poseidon &amp; Zeus)</t>
+  </si>
+  <si>
+    <t>Daedalus Hammer Augments - The Stygian Blade</t>
+  </si>
+  <si>
+    <t>Daedalus Hammer Augments - The Heart-Seeking Bow</t>
+  </si>
+  <si>
+    <t>Daedalus Hammer Augments - The Shield of Chaos</t>
+  </si>
+  <si>
+    <t>Daedalus Hammer Augments - The Eternal Spear</t>
+  </si>
+  <si>
+    <t>Daedalus Hammer Augments - The Twin Fists</t>
+  </si>
+  <si>
+    <t>Daedalus Hammer Augments - The Adamant Rail</t>
+  </si>
+  <si>
+    <t>Breaching Slash</t>
+  </si>
+  <si>
+    <t>Chain Shot</t>
+  </si>
+  <si>
+    <t>Breaching Rush</t>
+  </si>
+  <si>
+    <t>Breaching Skewer</t>
+  </si>
+  <si>
+    <t>Breaching Cross</t>
+  </si>
+  <si>
+    <t>Cluster Bomb</t>
+  </si>
+  <si>
+    <t>Cruel Thrust</t>
+  </si>
+  <si>
+    <t>Charged Volley</t>
+  </si>
+  <si>
+    <t>Charged Flight</t>
+  </si>
+  <si>
+    <t>Chain Skewer</t>
+  </si>
+  <si>
+    <t>Colossus Knuckle</t>
+  </si>
+  <si>
+    <t>Delta Chamber</t>
+  </si>
+  <si>
+    <t>Cursed Slash</t>
+  </si>
+  <si>
+    <t>Concentrated Volley</t>
+  </si>
+  <si>
+    <t>Charged Shot</t>
+  </si>
+  <si>
+    <t>Charged Skewer</t>
+  </si>
+  <si>
+    <t>Concentrated Knuckle</t>
+  </si>
+  <si>
+    <t>Explosive Fire</t>
+  </si>
+  <si>
+    <t>Double Edge</t>
+  </si>
+  <si>
+    <t>Explosive Shot</t>
+  </si>
+  <si>
+    <t>Dashing Flight</t>
+  </si>
+  <si>
+    <t>Exploding Launcher</t>
+  </si>
+  <si>
+    <t>Draining Cutter</t>
+  </si>
+  <si>
+    <t>Flurry Fire</t>
+  </si>
+  <si>
+    <t>Double Nova</t>
+  </si>
+  <si>
+    <t>Flurry Shot</t>
+  </si>
+  <si>
+    <t>Dashing Wallop</t>
+  </si>
+  <si>
+    <t>Extending Jab</t>
+  </si>
+  <si>
+    <t>Explosive Upper</t>
+  </si>
+  <si>
+    <t>Hazard Bomb</t>
+  </si>
+  <si>
+    <t>Flurry Slash</t>
+  </si>
+  <si>
+    <t>Perfect Shot</t>
+  </si>
+  <si>
+    <t>Dread Flight</t>
+  </si>
+  <si>
+    <t>Flaring Spin</t>
+  </si>
+  <si>
+    <t>Flying Cutter</t>
+  </si>
+  <si>
+    <t>Piercing Fire</t>
+  </si>
+  <si>
+    <t>Hoarding Slash</t>
+  </si>
+  <si>
+    <t>Piercing Volley</t>
+  </si>
+  <si>
+    <t>Empowering Flight</t>
+  </si>
+  <si>
+    <t>Flurry Jab</t>
+  </si>
+  <si>
+    <t>Heavy Knuckle</t>
+  </si>
+  <si>
+    <t>Ricochet Fire</t>
+  </si>
+  <si>
+    <t>Piercing Wave</t>
+  </si>
+  <si>
+    <t>Point-Blank Shot</t>
+  </si>
+  <si>
+    <t>Explosive Return</t>
+  </si>
+  <si>
+    <t>Massive Spin</t>
+  </si>
+  <si>
+    <t>Kinetic Launcher</t>
+  </si>
+  <si>
+    <t>Rocket Bomb</t>
+  </si>
+  <si>
+    <t>Shadow Slash</t>
+  </si>
+  <si>
+    <t>Relentless Volley</t>
+  </si>
+  <si>
+    <t>Ferocious Guard</t>
+  </si>
+  <si>
+    <t>Quick Spin</t>
+  </si>
+  <si>
+    <t>Long Knuckle</t>
+  </si>
+  <si>
+    <t>Seeking Fire</t>
+  </si>
+  <si>
+    <t>Snap Nova</t>
+  </si>
+  <si>
+    <t>Sniper Shot</t>
+  </si>
+  <si>
+    <t>Minotaur Rush</t>
+  </si>
+  <si>
+    <t>Serrated Point</t>
+  </si>
+  <si>
+    <t>Quake Cutter</t>
+  </si>
+  <si>
+    <t>Spread Fire</t>
+  </si>
+  <si>
+    <t>Super Nova</t>
+  </si>
+  <si>
+    <t>Triple Shot</t>
+  </si>
+  <si>
+    <t>Pulverizing Blow</t>
+  </si>
+  <si>
+    <t>Triple Jab</t>
+  </si>
+  <si>
+    <t>Rolling Knuckle</t>
+  </si>
+  <si>
+    <t>Targeting System</t>
+  </si>
+  <si>
+    <t>World Splitter</t>
+  </si>
+  <si>
+    <t>Twin Shot</t>
+  </si>
+  <si>
+    <t>Sudden Rush</t>
+  </si>
+  <si>
+    <t>Vicious Skewer</t>
+  </si>
+  <si>
+    <t>Rush Kick</t>
+  </si>
+  <si>
+    <t>Triple Bomb</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1728,11 +2508,13 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <name val="Aptos Narrow"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1740,6 +2522,7 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1753,6 +2536,29 @@
       <b/>
       <sz val="12"/>
       <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF242424"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1764,7 +2570,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -1772,17 +2578,36 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2117,70 +2942,70 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4659E671-0874-FE42-985B-794BDDF20B74}">
-  <dimension ref="A1:BB75"/>
+  <dimension ref="A1:CJ75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BC1" workbookViewId="0">
-      <selection activeCell="AE19" sqref="AE19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8515625" defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.5546875" customWidth="1"/>
-    <col min="2" max="2" width="6.53515625" customWidth="1"/>
-    <col min="3" max="3" width="21.703125" customWidth="1"/>
-    <col min="4" max="4" width="6.53515625" customWidth="1"/>
-    <col min="5" max="5" width="32.18359375" customWidth="1"/>
-    <col min="6" max="6" width="7.64453125" customWidth="1"/>
-    <col min="7" max="7" width="22.44140625" customWidth="1"/>
-    <col min="8" max="8" width="6.65625" customWidth="1"/>
-    <col min="9" max="9" width="21.82421875" customWidth="1"/>
-    <col min="10" max="10" width="7.02734375" customWidth="1"/>
-    <col min="11" max="11" width="29.1015625" customWidth="1"/>
-    <col min="12" max="12" width="8.13671875" customWidth="1"/>
-    <col min="13" max="13" width="21.703125" customWidth="1"/>
-    <col min="14" max="14" width="8.01171875" customWidth="1"/>
-    <col min="15" max="15" width="23.3046875" customWidth="1"/>
-    <col min="16" max="16" width="7.765625" customWidth="1"/>
-    <col min="17" max="17" width="21.703125" customWidth="1"/>
-    <col min="18" max="18" width="8.5078125" customWidth="1"/>
-    <col min="19" max="19" width="16.27734375" customWidth="1"/>
-    <col min="20" max="20" width="7.765625" customWidth="1"/>
-    <col min="22" max="22" width="8.3828125" customWidth="1"/>
-    <col min="23" max="23" width="16.27734375" customWidth="1"/>
-    <col min="24" max="24" width="6.78125" customWidth="1"/>
-    <col min="25" max="25" width="21.703125" customWidth="1"/>
-    <col min="26" max="26" width="7.51953125" customWidth="1"/>
-    <col min="27" max="27" width="21.453125" customWidth="1"/>
-    <col min="28" max="28" width="6.65625" customWidth="1"/>
-    <col min="29" max="29" width="21.703125" customWidth="1"/>
-    <col min="30" max="30" width="7.02734375" customWidth="1"/>
-    <col min="31" max="31" width="22.31640625" customWidth="1"/>
-    <col min="32" max="32" width="7.1484375" customWidth="1"/>
-    <col min="33" max="33" width="25.15234375" customWidth="1"/>
-    <col min="34" max="34" width="7.51953125" customWidth="1"/>
-    <col min="35" max="35" width="24.16796875" customWidth="1"/>
-    <col min="36" max="36" width="7.2734375" customWidth="1"/>
-    <col min="37" max="37" width="26.51171875" customWidth="1"/>
-    <col min="38" max="38" width="8.5078125" customWidth="1"/>
-    <col min="39" max="39" width="21.703125" customWidth="1"/>
-    <col min="40" max="40" width="8.3828125" customWidth="1"/>
-    <col min="41" max="41" width="26.015625" customWidth="1"/>
-    <col min="42" max="42" width="7.51953125" customWidth="1"/>
-    <col min="43" max="43" width="32.67578125" customWidth="1"/>
-    <col min="44" max="44" width="7.2734375" customWidth="1"/>
-    <col min="45" max="45" width="32.5546875" customWidth="1"/>
-    <col min="46" max="46" width="6.65625" customWidth="1"/>
-    <col min="47" max="47" width="32.67578125" customWidth="1"/>
-    <col min="48" max="48" width="7.51953125" customWidth="1"/>
-    <col min="49" max="49" width="32.3046875" customWidth="1"/>
-    <col min="50" max="50" width="6.65625" customWidth="1"/>
-    <col min="51" max="51" width="32.5546875" customWidth="1"/>
-    <col min="52" max="52" width="7.64453125" customWidth="1"/>
-    <col min="53" max="53" width="32.3046875" customWidth="1"/>
-    <col min="54" max="54" width="7.51953125" customWidth="1"/>
+    <col min="1" max="1" width="32.5" customWidth="1"/>
+    <col min="2" max="2" width="6.5" customWidth="1"/>
+    <col min="3" max="3" width="21.75" customWidth="1"/>
+    <col min="4" max="4" width="6.5" customWidth="1"/>
+    <col min="5" max="5" width="32.125" customWidth="1"/>
+    <col min="6" max="6" width="7.625" customWidth="1"/>
+    <col min="7" max="7" width="22.5" customWidth="1"/>
+    <col min="8" max="8" width="6.625" customWidth="1"/>
+    <col min="9" max="9" width="21.875" customWidth="1"/>
+    <col min="10" max="10" width="7" customWidth="1"/>
+    <col min="11" max="11" width="29.125" customWidth="1"/>
+    <col min="12" max="12" width="8.125" customWidth="1"/>
+    <col min="13" max="13" width="21.75" customWidth="1"/>
+    <col min="14" max="14" width="8" customWidth="1"/>
+    <col min="15" max="15" width="23.25" customWidth="1"/>
+    <col min="16" max="16" width="7.75" customWidth="1"/>
+    <col min="17" max="17" width="21.75" customWidth="1"/>
+    <col min="18" max="18" width="8.5" customWidth="1"/>
+    <col min="19" max="19" width="16.25" customWidth="1"/>
+    <col min="20" max="20" width="7.75" customWidth="1"/>
+    <col min="22" max="22" width="8.375" customWidth="1"/>
+    <col min="23" max="23" width="16.25" customWidth="1"/>
+    <col min="24" max="24" width="6.75" customWidth="1"/>
+    <col min="25" max="25" width="21.75" customWidth="1"/>
+    <col min="26" max="26" width="7.5" customWidth="1"/>
+    <col min="27" max="27" width="21.5" customWidth="1"/>
+    <col min="28" max="28" width="6.625" customWidth="1"/>
+    <col min="29" max="29" width="21.75" customWidth="1"/>
+    <col min="30" max="30" width="7" customWidth="1"/>
+    <col min="31" max="31" width="22.375" customWidth="1"/>
+    <col min="32" max="32" width="7.125" customWidth="1"/>
+    <col min="33" max="33" width="25.125" customWidth="1"/>
+    <col min="34" max="34" width="7.5" customWidth="1"/>
+    <col min="35" max="35" width="24.125" customWidth="1"/>
+    <col min="36" max="36" width="7.25" customWidth="1"/>
+    <col min="37" max="37" width="26.5" customWidth="1"/>
+    <col min="38" max="38" width="8.5" customWidth="1"/>
+    <col min="39" max="39" width="21.75" customWidth="1"/>
+    <col min="40" max="40" width="8.375" customWidth="1"/>
+    <col min="41" max="41" width="26" customWidth="1"/>
+    <col min="42" max="42" width="7.5" customWidth="1"/>
+    <col min="43" max="43" width="32.625" customWidth="1"/>
+    <col min="44" max="44" width="7.25" customWidth="1"/>
+    <col min="45" max="45" width="32.5" customWidth="1"/>
+    <col min="46" max="46" width="6.625" customWidth="1"/>
+    <col min="47" max="47" width="32.625" customWidth="1"/>
+    <col min="48" max="48" width="7.5" customWidth="1"/>
+    <col min="49" max="49" width="32.25" customWidth="1"/>
+    <col min="50" max="50" width="6.625" customWidth="1"/>
+    <col min="51" max="51" width="32.5" customWidth="1"/>
+    <col min="52" max="52" width="7.625" customWidth="1"/>
+    <col min="53" max="53" width="32.25" customWidth="1"/>
+    <col min="54" max="54" width="7.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:88" s="3" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2262,8 +3087,97 @@
       <c r="BA1" s="3" t="s">
         <v>347</v>
       </c>
+      <c r="BB1" s="6"/>
+      <c r="BC1" s="7" t="s">
+        <v>558</v>
+      </c>
+      <c r="BD1" s="7" t="s">
+        <v>559</v>
+      </c>
+      <c r="BE1" s="7" t="s">
+        <v>560</v>
+      </c>
+      <c r="BF1" s="7" t="s">
+        <v>559</v>
+      </c>
+      <c r="BG1" s="7" t="s">
+        <v>561</v>
+      </c>
+      <c r="BH1" s="7" t="s">
+        <v>559</v>
+      </c>
+      <c r="BI1" s="7" t="s">
+        <v>562</v>
+      </c>
+      <c r="BJ1" s="7" t="s">
+        <v>559</v>
+      </c>
+      <c r="BK1" s="7" t="s">
+        <v>563</v>
+      </c>
+      <c r="BL1" s="7" t="s">
+        <v>559</v>
+      </c>
+      <c r="BM1" s="7" t="s">
+        <v>564</v>
+      </c>
+      <c r="BN1" s="7" t="s">
+        <v>559</v>
+      </c>
+      <c r="BO1" s="7" t="s">
+        <v>565</v>
+      </c>
+      <c r="BP1" s="7" t="s">
+        <v>559</v>
+      </c>
+      <c r="BQ1" s="7" t="s">
+        <v>566</v>
+      </c>
+      <c r="BR1" s="7" t="s">
+        <v>559</v>
+      </c>
+      <c r="BS1" s="7" t="s">
+        <v>567</v>
+      </c>
+      <c r="BT1" s="7" t="s">
+        <v>559</v>
+      </c>
+      <c r="BU1" s="7" t="s">
+        <v>568</v>
+      </c>
+      <c r="BV1" s="7" t="s">
+        <v>559</v>
+      </c>
+      <c r="BW1" s="7" t="s">
+        <v>569</v>
+      </c>
+      <c r="BX1" s="6"/>
+      <c r="BY1" s="13" t="s">
+        <v>740</v>
+      </c>
+      <c r="BZ1" s="13"/>
+      <c r="CA1" s="13" t="s">
+        <v>741</v>
+      </c>
+      <c r="CB1" s="13"/>
+      <c r="CC1" s="12" t="s">
+        <v>742</v>
+      </c>
+      <c r="CD1" s="13"/>
+      <c r="CE1" s="12" t="s">
+        <v>743</v>
+      </c>
+      <c r="CF1" s="13"/>
+      <c r="CG1" s="12" t="s">
+        <v>744</v>
+      </c>
+      <c r="CH1" s="13"/>
+      <c r="CI1" s="12" t="s">
+        <v>745</v>
+      </c>
+      <c r="CJ1" s="13"/>
     </row>
-    <row r="2" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
@@ -2423,11 +3337,113 @@
       <c r="BA2" t="s">
         <v>348</v>
       </c>
-      <c r="BB2" s="4">
+      <c r="BB2" s="8">
+        <v>1</v>
+      </c>
+      <c r="BC2" s="9" t="s">
+        <v>570</v>
+      </c>
+      <c r="BD2" s="10">
+        <v>1</v>
+      </c>
+      <c r="BE2" s="9" t="s">
+        <v>571</v>
+      </c>
+      <c r="BF2" s="10">
+        <v>1</v>
+      </c>
+      <c r="BG2" s="9" t="s">
+        <v>572</v>
+      </c>
+      <c r="BH2" s="10">
+        <v>1</v>
+      </c>
+      <c r="BI2" s="9" t="s">
+        <v>573</v>
+      </c>
+      <c r="BJ2" s="10">
+        <v>1</v>
+      </c>
+      <c r="BK2" s="9" t="s">
+        <v>574</v>
+      </c>
+      <c r="BL2" s="10">
+        <v>1</v>
+      </c>
+      <c r="BM2" s="9" t="s">
+        <v>575</v>
+      </c>
+      <c r="BN2" s="10">
+        <v>1</v>
+      </c>
+      <c r="BO2" s="9" t="s">
+        <v>576</v>
+      </c>
+      <c r="BP2" s="10">
+        <v>1</v>
+      </c>
+      <c r="BQ2" s="9" t="s">
+        <v>577</v>
+      </c>
+      <c r="BR2" s="10">
+        <v>1</v>
+      </c>
+      <c r="BS2" s="9" t="s">
+        <v>578</v>
+      </c>
+      <c r="BT2" s="10">
+        <v>1</v>
+      </c>
+      <c r="BU2" s="9" t="s">
+        <v>579</v>
+      </c>
+      <c r="BV2" s="10">
+        <v>1</v>
+      </c>
+      <c r="BW2" s="10" t="s">
+        <v>580</v>
+      </c>
+      <c r="BX2" s="10">
+        <v>1</v>
+      </c>
+      <c r="BY2" t="s">
+        <v>746</v>
+      </c>
+      <c r="BZ2">
+        <v>1</v>
+      </c>
+      <c r="CA2" t="s">
+        <v>747</v>
+      </c>
+      <c r="CB2">
+        <v>1</v>
+      </c>
+      <c r="CC2" t="s">
+        <v>748</v>
+      </c>
+      <c r="CD2">
+        <v>1</v>
+      </c>
+      <c r="CE2" t="s">
+        <v>749</v>
+      </c>
+      <c r="CF2">
+        <v>1</v>
+      </c>
+      <c r="CG2" t="s">
+        <v>750</v>
+      </c>
+      <c r="CH2">
+        <v>1</v>
+      </c>
+      <c r="CI2" t="s">
+        <v>751</v>
+      </c>
+      <c r="CJ2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>2</v>
       </c>
@@ -2587,11 +3603,113 @@
       <c r="BA3" t="s">
         <v>349</v>
       </c>
-      <c r="BB3" s="4">
+      <c r="BB3" s="8">
+        <v>1</v>
+      </c>
+      <c r="BC3" s="9" t="s">
+        <v>581</v>
+      </c>
+      <c r="BD3" s="10">
+        <v>1</v>
+      </c>
+      <c r="BE3" s="9" t="s">
+        <v>582</v>
+      </c>
+      <c r="BF3" s="10">
+        <v>1</v>
+      </c>
+      <c r="BG3" s="9" t="s">
+        <v>583</v>
+      </c>
+      <c r="BH3" s="10">
+        <v>1</v>
+      </c>
+      <c r="BI3" s="9" t="s">
+        <v>584</v>
+      </c>
+      <c r="BJ3" s="10">
+        <v>1</v>
+      </c>
+      <c r="BK3" s="9" t="s">
+        <v>585</v>
+      </c>
+      <c r="BL3" s="10">
+        <v>1</v>
+      </c>
+      <c r="BM3" s="9" t="s">
+        <v>586</v>
+      </c>
+      <c r="BN3" s="10">
+        <v>1</v>
+      </c>
+      <c r="BO3" s="9" t="s">
+        <v>587</v>
+      </c>
+      <c r="BP3" s="10">
+        <v>1</v>
+      </c>
+      <c r="BQ3" s="9" t="s">
+        <v>588</v>
+      </c>
+      <c r="BR3" s="10">
+        <v>1</v>
+      </c>
+      <c r="BS3" s="9" t="s">
+        <v>589</v>
+      </c>
+      <c r="BT3" s="10">
+        <v>1</v>
+      </c>
+      <c r="BU3" s="9" t="s">
+        <v>590</v>
+      </c>
+      <c r="BV3" s="10">
+        <v>1</v>
+      </c>
+      <c r="BW3" s="10" t="s">
+        <v>591</v>
+      </c>
+      <c r="BX3" s="10">
+        <v>1</v>
+      </c>
+      <c r="BY3" t="s">
+        <v>752</v>
+      </c>
+      <c r="BZ3">
+        <v>1</v>
+      </c>
+      <c r="CA3" t="s">
+        <v>753</v>
+      </c>
+      <c r="CB3">
+        <v>1</v>
+      </c>
+      <c r="CC3" t="s">
+        <v>754</v>
+      </c>
+      <c r="CD3">
+        <v>1</v>
+      </c>
+      <c r="CE3" t="s">
+        <v>755</v>
+      </c>
+      <c r="CF3">
+        <v>1</v>
+      </c>
+      <c r="CG3" t="s">
+        <v>756</v>
+      </c>
+      <c r="CH3">
+        <v>1</v>
+      </c>
+      <c r="CI3" t="s">
+        <v>757</v>
+      </c>
+      <c r="CJ3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>3</v>
       </c>
@@ -2751,11 +3869,113 @@
       <c r="BA4" t="s">
         <v>350</v>
       </c>
-      <c r="BB4" s="4">
+      <c r="BB4" s="8">
+        <v>1</v>
+      </c>
+      <c r="BC4" s="9" t="s">
+        <v>592</v>
+      </c>
+      <c r="BD4" s="10">
+        <v>1</v>
+      </c>
+      <c r="BE4" s="9" t="s">
+        <v>593</v>
+      </c>
+      <c r="BF4" s="10">
+        <v>1</v>
+      </c>
+      <c r="BG4" s="9" t="s">
+        <v>594</v>
+      </c>
+      <c r="BH4" s="10">
+        <v>1</v>
+      </c>
+      <c r="BI4" s="9" t="s">
+        <v>595</v>
+      </c>
+      <c r="BJ4" s="10">
+        <v>1</v>
+      </c>
+      <c r="BK4" s="9" t="s">
+        <v>596</v>
+      </c>
+      <c r="BL4" s="10">
+        <v>1</v>
+      </c>
+      <c r="BM4" s="9" t="s">
+        <v>597</v>
+      </c>
+      <c r="BN4" s="10">
+        <v>1</v>
+      </c>
+      <c r="BO4" s="9" t="s">
+        <v>598</v>
+      </c>
+      <c r="BP4" s="10">
+        <v>1</v>
+      </c>
+      <c r="BQ4" s="9" t="s">
+        <v>599</v>
+      </c>
+      <c r="BR4" s="10">
+        <v>1</v>
+      </c>
+      <c r="BS4" s="9" t="s">
+        <v>600</v>
+      </c>
+      <c r="BT4" s="10">
+        <v>1</v>
+      </c>
+      <c r="BU4" s="9" t="s">
+        <v>601</v>
+      </c>
+      <c r="BV4" s="10">
+        <v>1</v>
+      </c>
+      <c r="BW4" s="10" t="s">
+        <v>602</v>
+      </c>
+      <c r="BX4" s="10">
+        <v>1</v>
+      </c>
+      <c r="BY4" t="s">
+        <v>758</v>
+      </c>
+      <c r="BZ4">
+        <v>1</v>
+      </c>
+      <c r="CA4" t="s">
+        <v>759</v>
+      </c>
+      <c r="CB4">
+        <v>1</v>
+      </c>
+      <c r="CC4" t="s">
+        <v>760</v>
+      </c>
+      <c r="CD4">
+        <v>1</v>
+      </c>
+      <c r="CE4" t="s">
+        <v>761</v>
+      </c>
+      <c r="CF4">
+        <v>1</v>
+      </c>
+      <c r="CG4" t="s">
+        <v>762</v>
+      </c>
+      <c r="CH4">
+        <v>1</v>
+      </c>
+      <c r="CI4" t="s">
+        <v>763</v>
+      </c>
+      <c r="CJ4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>4</v>
       </c>
@@ -2915,11 +4135,113 @@
       <c r="BA5" t="s">
         <v>351</v>
       </c>
-      <c r="BB5" s="4">
+      <c r="BB5" s="8">
+        <v>1</v>
+      </c>
+      <c r="BC5" s="9" t="s">
+        <v>603</v>
+      </c>
+      <c r="BD5" s="10">
+        <v>1</v>
+      </c>
+      <c r="BE5" s="9" t="s">
+        <v>604</v>
+      </c>
+      <c r="BF5" s="10">
+        <v>1</v>
+      </c>
+      <c r="BG5" s="9" t="s">
+        <v>605</v>
+      </c>
+      <c r="BH5" s="10">
+        <v>1</v>
+      </c>
+      <c r="BI5" s="9" t="s">
+        <v>606</v>
+      </c>
+      <c r="BJ5" s="10">
+        <v>1</v>
+      </c>
+      <c r="BK5" s="9" t="s">
+        <v>607</v>
+      </c>
+      <c r="BL5" s="10">
+        <v>1</v>
+      </c>
+      <c r="BM5" s="9" t="s">
+        <v>608</v>
+      </c>
+      <c r="BN5" s="10">
+        <v>1</v>
+      </c>
+      <c r="BO5" s="9" t="s">
+        <v>609</v>
+      </c>
+      <c r="BP5" s="10">
+        <v>1</v>
+      </c>
+      <c r="BQ5" s="9" t="s">
+        <v>610</v>
+      </c>
+      <c r="BR5" s="10">
+        <v>1</v>
+      </c>
+      <c r="BS5" s="9" t="s">
+        <v>611</v>
+      </c>
+      <c r="BT5" s="10">
+        <v>1</v>
+      </c>
+      <c r="BU5" s="9" t="s">
+        <v>612</v>
+      </c>
+      <c r="BV5" s="10">
+        <v>1</v>
+      </c>
+      <c r="BW5" s="10" t="s">
+        <v>613</v>
+      </c>
+      <c r="BX5" s="10">
+        <v>1</v>
+      </c>
+      <c r="BY5" t="s">
+        <v>764</v>
+      </c>
+      <c r="BZ5">
+        <v>1</v>
+      </c>
+      <c r="CA5" t="s">
+        <v>765</v>
+      </c>
+      <c r="CB5">
+        <v>1</v>
+      </c>
+      <c r="CC5" t="s">
+        <v>766</v>
+      </c>
+      <c r="CD5">
+        <v>1</v>
+      </c>
+      <c r="CE5" t="s">
+        <v>767</v>
+      </c>
+      <c r="CF5">
+        <v>1</v>
+      </c>
+      <c r="CG5" t="s">
+        <v>768</v>
+      </c>
+      <c r="CH5">
+        <v>1</v>
+      </c>
+      <c r="CI5" t="s">
+        <v>769</v>
+      </c>
+      <c r="CJ5">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:54" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:88" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>5</v>
       </c>
@@ -3079,11 +4401,113 @@
       <c r="BA6" t="s">
         <v>352</v>
       </c>
-      <c r="BB6" s="4">
+      <c r="BB6" s="8">
+        <v>1</v>
+      </c>
+      <c r="BC6" s="9" t="s">
+        <v>614</v>
+      </c>
+      <c r="BD6" s="10">
+        <v>1</v>
+      </c>
+      <c r="BE6" s="9" t="s">
+        <v>615</v>
+      </c>
+      <c r="BF6" s="10">
+        <v>1</v>
+      </c>
+      <c r="BG6" s="9" t="s">
+        <v>616</v>
+      </c>
+      <c r="BH6" s="10">
+        <v>1</v>
+      </c>
+      <c r="BI6" s="9" t="s">
+        <v>617</v>
+      </c>
+      <c r="BJ6" s="10">
+        <v>1</v>
+      </c>
+      <c r="BK6" s="9" t="s">
+        <v>618</v>
+      </c>
+      <c r="BL6" s="10">
+        <v>1</v>
+      </c>
+      <c r="BM6" s="9" t="s">
+        <v>619</v>
+      </c>
+      <c r="BN6" s="10">
+        <v>1</v>
+      </c>
+      <c r="BO6" s="9" t="s">
+        <v>620</v>
+      </c>
+      <c r="BP6" s="10">
+        <v>1</v>
+      </c>
+      <c r="BQ6" s="9" t="s">
+        <v>621</v>
+      </c>
+      <c r="BR6" s="10">
+        <v>1</v>
+      </c>
+      <c r="BS6" s="9" t="s">
+        <v>622</v>
+      </c>
+      <c r="BT6" s="10">
+        <v>1</v>
+      </c>
+      <c r="BU6" s="9" t="s">
+        <v>623</v>
+      </c>
+      <c r="BV6" s="10">
+        <v>1</v>
+      </c>
+      <c r="BW6" s="10" t="s">
+        <v>624</v>
+      </c>
+      <c r="BX6" s="10">
+        <v>1</v>
+      </c>
+      <c r="BY6" t="s">
+        <v>770</v>
+      </c>
+      <c r="BZ6">
+        <v>1</v>
+      </c>
+      <c r="CA6" t="s">
+        <v>771</v>
+      </c>
+      <c r="CB6">
+        <v>1</v>
+      </c>
+      <c r="CC6" t="s">
+        <v>772</v>
+      </c>
+      <c r="CD6">
+        <v>1</v>
+      </c>
+      <c r="CE6" t="s">
+        <v>773</v>
+      </c>
+      <c r="CF6">
+        <v>1</v>
+      </c>
+      <c r="CG6" t="s">
+        <v>774</v>
+      </c>
+      <c r="CH6">
+        <v>1</v>
+      </c>
+      <c r="CI6" t="s">
+        <v>775</v>
+      </c>
+      <c r="CJ6">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>6</v>
       </c>
@@ -3213,11 +4637,113 @@
       <c r="BA7" t="s">
         <v>353</v>
       </c>
-      <c r="BB7" s="4">
+      <c r="BB7" s="8">
+        <v>1</v>
+      </c>
+      <c r="BC7" s="9" t="s">
+        <v>625</v>
+      </c>
+      <c r="BD7" s="10">
+        <v>1</v>
+      </c>
+      <c r="BE7" s="9" t="s">
+        <v>626</v>
+      </c>
+      <c r="BF7" s="10">
+        <v>1</v>
+      </c>
+      <c r="BG7" s="9" t="s">
+        <v>627</v>
+      </c>
+      <c r="BH7" s="10">
+        <v>1</v>
+      </c>
+      <c r="BI7" s="9" t="s">
+        <v>628</v>
+      </c>
+      <c r="BJ7" s="10">
+        <v>1</v>
+      </c>
+      <c r="BK7" s="9" t="s">
+        <v>629</v>
+      </c>
+      <c r="BL7" s="10">
+        <v>1</v>
+      </c>
+      <c r="BM7" s="9" t="s">
+        <v>630</v>
+      </c>
+      <c r="BN7" s="10">
+        <v>1</v>
+      </c>
+      <c r="BO7" s="9" t="s">
+        <v>631</v>
+      </c>
+      <c r="BP7" s="10">
+        <v>1</v>
+      </c>
+      <c r="BQ7" s="9" t="s">
+        <v>632</v>
+      </c>
+      <c r="BR7" s="10">
+        <v>1</v>
+      </c>
+      <c r="BS7" s="9" t="s">
+        <v>633</v>
+      </c>
+      <c r="BT7" s="10">
+        <v>1</v>
+      </c>
+      <c r="BU7" s="9" t="s">
+        <v>634</v>
+      </c>
+      <c r="BV7" s="10">
+        <v>1</v>
+      </c>
+      <c r="BW7" s="10" t="s">
+        <v>635</v>
+      </c>
+      <c r="BX7" s="10">
+        <v>1</v>
+      </c>
+      <c r="BY7" t="s">
+        <v>776</v>
+      </c>
+      <c r="BZ7">
+        <v>1</v>
+      </c>
+      <c r="CA7" t="s">
+        <v>777</v>
+      </c>
+      <c r="CB7">
+        <v>1</v>
+      </c>
+      <c r="CC7" t="s">
+        <v>778</v>
+      </c>
+      <c r="CD7">
+        <v>1</v>
+      </c>
+      <c r="CE7" t="s">
+        <v>779</v>
+      </c>
+      <c r="CF7">
+        <v>1</v>
+      </c>
+      <c r="CG7" t="s">
+        <v>780</v>
+      </c>
+      <c r="CH7">
+        <v>1</v>
+      </c>
+      <c r="CI7" t="s">
+        <v>781</v>
+      </c>
+      <c r="CJ7">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>17</v>
       </c>
@@ -3343,11 +4869,113 @@
       <c r="BA8" t="s">
         <v>354</v>
       </c>
-      <c r="BB8" s="4">
+      <c r="BB8" s="8">
+        <v>1</v>
+      </c>
+      <c r="BC8" s="9" t="s">
+        <v>636</v>
+      </c>
+      <c r="BD8" s="10">
+        <v>1</v>
+      </c>
+      <c r="BE8" s="9" t="s">
+        <v>637</v>
+      </c>
+      <c r="BF8" s="10">
+        <v>1</v>
+      </c>
+      <c r="BG8" s="9" t="s">
+        <v>638</v>
+      </c>
+      <c r="BH8" s="10">
+        <v>1</v>
+      </c>
+      <c r="BI8" s="9" t="s">
+        <v>639</v>
+      </c>
+      <c r="BJ8" s="10">
+        <v>1</v>
+      </c>
+      <c r="BK8" s="9" t="s">
+        <v>640</v>
+      </c>
+      <c r="BL8" s="10">
+        <v>1</v>
+      </c>
+      <c r="BM8" s="9" t="s">
+        <v>641</v>
+      </c>
+      <c r="BN8" s="10">
+        <v>1</v>
+      </c>
+      <c r="BO8" s="9" t="s">
+        <v>642</v>
+      </c>
+      <c r="BP8" s="10">
+        <v>1</v>
+      </c>
+      <c r="BQ8" s="9" t="s">
+        <v>643</v>
+      </c>
+      <c r="BR8" s="10">
+        <v>1</v>
+      </c>
+      <c r="BS8" s="9" t="s">
+        <v>644</v>
+      </c>
+      <c r="BT8" s="10">
+        <v>1</v>
+      </c>
+      <c r="BU8" s="9" t="s">
+        <v>645</v>
+      </c>
+      <c r="BV8" s="10">
+        <v>1</v>
+      </c>
+      <c r="BW8" s="10" t="s">
+        <v>646</v>
+      </c>
+      <c r="BX8" s="10">
+        <v>1</v>
+      </c>
+      <c r="BY8" t="s">
+        <v>782</v>
+      </c>
+      <c r="BZ8">
+        <v>1</v>
+      </c>
+      <c r="CA8" t="s">
+        <v>783</v>
+      </c>
+      <c r="CB8">
+        <v>1</v>
+      </c>
+      <c r="CC8" t="s">
+        <v>784</v>
+      </c>
+      <c r="CD8">
+        <v>1</v>
+      </c>
+      <c r="CE8" t="s">
+        <v>785</v>
+      </c>
+      <c r="CF8">
+        <v>1</v>
+      </c>
+      <c r="CG8" t="s">
+        <v>786</v>
+      </c>
+      <c r="CH8">
+        <v>1</v>
+      </c>
+      <c r="CI8" t="s">
+        <v>787</v>
+      </c>
+      <c r="CJ8">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>7</v>
       </c>
@@ -3467,11 +5095,113 @@
       <c r="BA9" t="s">
         <v>355</v>
       </c>
-      <c r="BB9" s="4">
+      <c r="BB9" s="8">
+        <v>1</v>
+      </c>
+      <c r="BC9" s="9" t="s">
+        <v>647</v>
+      </c>
+      <c r="BD9" s="10">
+        <v>1</v>
+      </c>
+      <c r="BE9" s="9" t="s">
+        <v>648</v>
+      </c>
+      <c r="BF9" s="10">
+        <v>1</v>
+      </c>
+      <c r="BG9" s="9" t="s">
+        <v>649</v>
+      </c>
+      <c r="BH9" s="10">
+        <v>1</v>
+      </c>
+      <c r="BI9" s="9" t="s">
+        <v>650</v>
+      </c>
+      <c r="BJ9" s="10">
+        <v>1</v>
+      </c>
+      <c r="BK9" s="9" t="s">
+        <v>651</v>
+      </c>
+      <c r="BL9" s="10">
+        <v>1</v>
+      </c>
+      <c r="BM9" s="9" t="s">
+        <v>652</v>
+      </c>
+      <c r="BN9" s="10">
+        <v>1</v>
+      </c>
+      <c r="BO9" s="9" t="s">
+        <v>653</v>
+      </c>
+      <c r="BP9" s="10">
+        <v>1</v>
+      </c>
+      <c r="BQ9" s="9" t="s">
+        <v>654</v>
+      </c>
+      <c r="BR9" s="10">
+        <v>1</v>
+      </c>
+      <c r="BS9" s="9" t="s">
+        <v>655</v>
+      </c>
+      <c r="BT9" s="10">
+        <v>1</v>
+      </c>
+      <c r="BU9" s="9" t="s">
+        <v>656</v>
+      </c>
+      <c r="BV9" s="10">
+        <v>1</v>
+      </c>
+      <c r="BW9" s="10" t="s">
+        <v>657</v>
+      </c>
+      <c r="BX9" s="10">
+        <v>1</v>
+      </c>
+      <c r="BY9" t="s">
+        <v>788</v>
+      </c>
+      <c r="BZ9">
+        <v>1</v>
+      </c>
+      <c r="CA9" t="s">
+        <v>789</v>
+      </c>
+      <c r="CB9">
+        <v>1</v>
+      </c>
+      <c r="CC9" t="s">
+        <v>790</v>
+      </c>
+      <c r="CD9">
+        <v>1</v>
+      </c>
+      <c r="CE9" t="s">
+        <v>791</v>
+      </c>
+      <c r="CF9">
+        <v>1</v>
+      </c>
+      <c r="CG9" t="s">
+        <v>792</v>
+      </c>
+      <c r="CH9">
+        <v>1</v>
+      </c>
+      <c r="CI9" t="s">
+        <v>793</v>
+      </c>
+      <c r="CJ9">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>8</v>
       </c>
@@ -3591,11 +5321,113 @@
       <c r="BA10" t="s">
         <v>356</v>
       </c>
-      <c r="BB10" s="4">
+      <c r="BB10" s="8">
+        <v>1</v>
+      </c>
+      <c r="BC10" s="9" t="s">
+        <v>658</v>
+      </c>
+      <c r="BD10" s="10">
+        <v>1</v>
+      </c>
+      <c r="BE10" s="9" t="s">
+        <v>659</v>
+      </c>
+      <c r="BF10" s="10">
+        <v>1</v>
+      </c>
+      <c r="BG10" s="9" t="s">
+        <v>660</v>
+      </c>
+      <c r="BH10" s="10">
+        <v>1</v>
+      </c>
+      <c r="BI10" s="9" t="s">
+        <v>661</v>
+      </c>
+      <c r="BJ10" s="10">
+        <v>1</v>
+      </c>
+      <c r="BK10" s="9" t="s">
+        <v>662</v>
+      </c>
+      <c r="BL10" s="10">
+        <v>1</v>
+      </c>
+      <c r="BM10" s="9" t="s">
+        <v>663</v>
+      </c>
+      <c r="BN10" s="10">
+        <v>1</v>
+      </c>
+      <c r="BO10" s="9" t="s">
+        <v>664</v>
+      </c>
+      <c r="BP10" s="10">
+        <v>1</v>
+      </c>
+      <c r="BQ10" s="9" t="s">
+        <v>665</v>
+      </c>
+      <c r="BR10" s="10">
+        <v>1</v>
+      </c>
+      <c r="BS10" s="9" t="s">
+        <v>666</v>
+      </c>
+      <c r="BT10" s="10">
+        <v>1</v>
+      </c>
+      <c r="BU10" s="9" t="s">
+        <v>667</v>
+      </c>
+      <c r="BV10" s="10">
+        <v>1</v>
+      </c>
+      <c r="BW10" s="10" t="s">
+        <v>668</v>
+      </c>
+      <c r="BX10" s="10">
+        <v>1</v>
+      </c>
+      <c r="BY10" t="s">
+        <v>794</v>
+      </c>
+      <c r="BZ10">
+        <v>1</v>
+      </c>
+      <c r="CA10" t="s">
+        <v>795</v>
+      </c>
+      <c r="CB10">
+        <v>1</v>
+      </c>
+      <c r="CC10" t="s">
+        <v>796</v>
+      </c>
+      <c r="CD10">
+        <v>1</v>
+      </c>
+      <c r="CE10" t="s">
+        <v>797</v>
+      </c>
+      <c r="CF10">
+        <v>1</v>
+      </c>
+      <c r="CG10" t="s">
+        <v>798</v>
+      </c>
+      <c r="CH10">
+        <v>1</v>
+      </c>
+      <c r="CI10" t="s">
+        <v>799</v>
+      </c>
+      <c r="CJ10">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>9</v>
       </c>
@@ -3715,11 +5547,113 @@
       <c r="BA11" t="s">
         <v>357</v>
       </c>
-      <c r="BB11" s="4">
+      <c r="BB11" s="8">
+        <v>1</v>
+      </c>
+      <c r="BC11" s="9" t="s">
+        <v>669</v>
+      </c>
+      <c r="BD11" s="10">
+        <v>1</v>
+      </c>
+      <c r="BE11" s="9" t="s">
+        <v>670</v>
+      </c>
+      <c r="BF11" s="10">
+        <v>1</v>
+      </c>
+      <c r="BG11" s="9" t="s">
+        <v>671</v>
+      </c>
+      <c r="BH11" s="10">
+        <v>1</v>
+      </c>
+      <c r="BI11" s="9" t="s">
+        <v>672</v>
+      </c>
+      <c r="BJ11" s="10">
+        <v>1</v>
+      </c>
+      <c r="BK11" s="9" t="s">
+        <v>673</v>
+      </c>
+      <c r="BL11" s="10">
+        <v>1</v>
+      </c>
+      <c r="BM11" s="9" t="s">
+        <v>674</v>
+      </c>
+      <c r="BN11" s="10">
+        <v>1</v>
+      </c>
+      <c r="BO11" s="9" t="s">
+        <v>675</v>
+      </c>
+      <c r="BP11" s="10">
+        <v>1</v>
+      </c>
+      <c r="BQ11" s="9" t="s">
+        <v>676</v>
+      </c>
+      <c r="BR11" s="10">
+        <v>1</v>
+      </c>
+      <c r="BS11" s="9" t="s">
+        <v>677</v>
+      </c>
+      <c r="BT11" s="10">
+        <v>1</v>
+      </c>
+      <c r="BU11" s="9" t="s">
+        <v>678</v>
+      </c>
+      <c r="BV11" s="10">
+        <v>1</v>
+      </c>
+      <c r="BW11" s="10" t="s">
+        <v>679</v>
+      </c>
+      <c r="BX11" s="10">
+        <v>1</v>
+      </c>
+      <c r="BY11" t="s">
+        <v>800</v>
+      </c>
+      <c r="BZ11">
+        <v>1</v>
+      </c>
+      <c r="CA11" t="s">
+        <v>801</v>
+      </c>
+      <c r="CB11">
+        <v>1</v>
+      </c>
+      <c r="CC11" t="s">
+        <v>802</v>
+      </c>
+      <c r="CD11">
+        <v>1</v>
+      </c>
+      <c r="CE11" t="s">
+        <v>803</v>
+      </c>
+      <c r="CF11">
+        <v>1</v>
+      </c>
+      <c r="CG11" t="s">
+        <v>804</v>
+      </c>
+      <c r="CH11">
+        <v>1</v>
+      </c>
+      <c r="CI11" t="s">
+        <v>805</v>
+      </c>
+      <c r="CJ11">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>10</v>
       </c>
@@ -3834,11 +5768,113 @@
       <c r="BA12" t="s">
         <v>358</v>
       </c>
-      <c r="BB12" s="4">
+      <c r="BB12" s="8">
+        <v>1</v>
+      </c>
+      <c r="BC12" s="9" t="s">
+        <v>680</v>
+      </c>
+      <c r="BD12" s="10">
+        <v>1</v>
+      </c>
+      <c r="BE12" s="9" t="s">
+        <v>681</v>
+      </c>
+      <c r="BF12" s="10">
+        <v>1</v>
+      </c>
+      <c r="BG12" s="9" t="s">
+        <v>682</v>
+      </c>
+      <c r="BH12" s="10">
+        <v>1</v>
+      </c>
+      <c r="BI12" s="9" t="s">
+        <v>683</v>
+      </c>
+      <c r="BJ12" s="10">
+        <v>1</v>
+      </c>
+      <c r="BK12" s="9" t="s">
+        <v>684</v>
+      </c>
+      <c r="BL12" s="10">
+        <v>1</v>
+      </c>
+      <c r="BM12" s="11" t="s">
+        <v>685</v>
+      </c>
+      <c r="BN12" s="10">
+        <v>1</v>
+      </c>
+      <c r="BO12" s="9" t="s">
+        <v>686</v>
+      </c>
+      <c r="BP12" s="10">
+        <v>1</v>
+      </c>
+      <c r="BQ12" s="9" t="s">
+        <v>687</v>
+      </c>
+      <c r="BR12" s="10">
+        <v>1</v>
+      </c>
+      <c r="BS12" s="9" t="s">
+        <v>688</v>
+      </c>
+      <c r="BT12" s="10">
+        <v>1</v>
+      </c>
+      <c r="BU12" s="9" t="s">
+        <v>689</v>
+      </c>
+      <c r="BV12" s="10">
+        <v>1</v>
+      </c>
+      <c r="BW12" s="10" t="s">
+        <v>690</v>
+      </c>
+      <c r="BX12" s="10">
+        <v>1</v>
+      </c>
+      <c r="BY12" t="s">
+        <v>806</v>
+      </c>
+      <c r="BZ12">
+        <v>1</v>
+      </c>
+      <c r="CA12" t="s">
+        <v>807</v>
+      </c>
+      <c r="CB12">
+        <v>1</v>
+      </c>
+      <c r="CC12" t="s">
+        <v>808</v>
+      </c>
+      <c r="CD12">
+        <v>1</v>
+      </c>
+      <c r="CE12" t="s">
+        <v>809</v>
+      </c>
+      <c r="CF12">
+        <v>1</v>
+      </c>
+      <c r="CG12" t="s">
+        <v>810</v>
+      </c>
+      <c r="CH12">
+        <v>1</v>
+      </c>
+      <c r="CI12" t="s">
+        <v>811</v>
+      </c>
+      <c r="CJ12">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>11</v>
       </c>
@@ -3947,11 +5983,113 @@
       <c r="BA13" t="s">
         <v>359</v>
       </c>
-      <c r="BB13" s="4">
+      <c r="BB13" s="8">
+        <v>1</v>
+      </c>
+      <c r="BC13" s="9" t="s">
+        <v>691</v>
+      </c>
+      <c r="BD13" s="10">
+        <v>1</v>
+      </c>
+      <c r="BE13" s="9" t="s">
+        <v>692</v>
+      </c>
+      <c r="BF13" s="10">
+        <v>1</v>
+      </c>
+      <c r="BG13" s="9" t="s">
+        <v>693</v>
+      </c>
+      <c r="BH13" s="10">
+        <v>1</v>
+      </c>
+      <c r="BI13" s="9" t="s">
+        <v>694</v>
+      </c>
+      <c r="BJ13" s="10">
+        <v>1</v>
+      </c>
+      <c r="BK13" s="9" t="s">
+        <v>695</v>
+      </c>
+      <c r="BL13" s="10">
+        <v>1</v>
+      </c>
+      <c r="BM13" s="9" t="s">
+        <v>696</v>
+      </c>
+      <c r="BN13" s="10">
+        <v>1</v>
+      </c>
+      <c r="BO13" s="9" t="s">
+        <v>697</v>
+      </c>
+      <c r="BP13" s="10">
+        <v>1</v>
+      </c>
+      <c r="BQ13" s="9" t="s">
+        <v>698</v>
+      </c>
+      <c r="BR13" s="10">
+        <v>1</v>
+      </c>
+      <c r="BS13" s="9" t="s">
+        <v>699</v>
+      </c>
+      <c r="BT13" s="10">
+        <v>1</v>
+      </c>
+      <c r="BU13" s="9" t="s">
+        <v>700</v>
+      </c>
+      <c r="BV13" s="10">
+        <v>1</v>
+      </c>
+      <c r="BW13" s="10" t="s">
+        <v>701</v>
+      </c>
+      <c r="BX13" s="10">
+        <v>1</v>
+      </c>
+      <c r="BY13" t="s">
+        <v>812</v>
+      </c>
+      <c r="BZ13">
+        <v>1</v>
+      </c>
+      <c r="CA13" t="s">
+        <v>813</v>
+      </c>
+      <c r="CB13">
+        <v>1</v>
+      </c>
+      <c r="CC13" t="s">
+        <v>814</v>
+      </c>
+      <c r="CD13">
+        <v>1</v>
+      </c>
+      <c r="CE13" t="s">
+        <v>815</v>
+      </c>
+      <c r="CF13">
+        <v>1</v>
+      </c>
+      <c r="CG13" t="s">
+        <v>816</v>
+      </c>
+      <c r="CH13">
+        <v>1</v>
+      </c>
+      <c r="CI13" t="s">
+        <v>817</v>
+      </c>
+      <c r="CJ13">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>12</v>
       </c>
@@ -4048,11 +6186,69 @@
       <c r="BA14" t="s">
         <v>360</v>
       </c>
-      <c r="BB14" s="4">
+      <c r="BB14" s="8">
+        <v>1</v>
+      </c>
+      <c r="BC14" s="9" t="s">
+        <v>702</v>
+      </c>
+      <c r="BD14" s="10">
+        <v>1</v>
+      </c>
+      <c r="BE14" s="9" t="s">
+        <v>703</v>
+      </c>
+      <c r="BF14" s="10">
+        <v>1</v>
+      </c>
+      <c r="BG14" s="9" t="s">
+        <v>704</v>
+      </c>
+      <c r="BH14" s="10">
+        <v>1</v>
+      </c>
+      <c r="BI14" s="10"/>
+      <c r="BJ14" s="10"/>
+      <c r="BK14" s="10"/>
+      <c r="BL14" s="10"/>
+      <c r="BM14" s="9" t="s">
+        <v>705</v>
+      </c>
+      <c r="BN14" s="10">
+        <v>1</v>
+      </c>
+      <c r="BO14" s="9" t="s">
+        <v>706</v>
+      </c>
+      <c r="BP14" s="10">
+        <v>1</v>
+      </c>
+      <c r="BQ14" s="9" t="s">
+        <v>707</v>
+      </c>
+      <c r="BR14" s="10">
+        <v>1</v>
+      </c>
+      <c r="BS14" s="9" t="s">
+        <v>708</v>
+      </c>
+      <c r="BT14" s="10">
+        <v>1</v>
+      </c>
+      <c r="BU14" s="9" t="s">
+        <v>709</v>
+      </c>
+      <c r="BV14" s="10">
+        <v>1</v>
+      </c>
+      <c r="BW14" s="10" t="s">
+        <v>710</v>
+      </c>
+      <c r="BX14" s="10">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>13</v>
       </c>
@@ -4149,11 +6345,65 @@
       <c r="BA15" t="s">
         <v>361</v>
       </c>
-      <c r="BB15" s="4">
+      <c r="BB15" s="8">
+        <v>1</v>
+      </c>
+      <c r="BC15" s="9" t="s">
+        <v>711</v>
+      </c>
+      <c r="BD15" s="10">
+        <v>1</v>
+      </c>
+      <c r="BE15" s="9" t="s">
+        <v>712</v>
+      </c>
+      <c r="BF15" s="10">
+        <v>1</v>
+      </c>
+      <c r="BG15" s="10"/>
+      <c r="BH15" s="10"/>
+      <c r="BI15" s="10"/>
+      <c r="BJ15" s="10"/>
+      <c r="BK15" s="10"/>
+      <c r="BL15" s="10"/>
+      <c r="BM15" s="9" t="s">
+        <v>713</v>
+      </c>
+      <c r="BN15" s="10">
+        <v>1</v>
+      </c>
+      <c r="BO15" s="9" t="s">
+        <v>714</v>
+      </c>
+      <c r="BP15" s="10">
+        <v>1</v>
+      </c>
+      <c r="BQ15" s="9" t="s">
+        <v>715</v>
+      </c>
+      <c r="BR15" s="10">
+        <v>1</v>
+      </c>
+      <c r="BS15" s="9" t="s">
+        <v>716</v>
+      </c>
+      <c r="BT15" s="10">
+        <v>1</v>
+      </c>
+      <c r="BU15" s="9" t="s">
+        <v>717</v>
+      </c>
+      <c r="BV15" s="10">
+        <v>1</v>
+      </c>
+      <c r="BW15" s="10" t="s">
+        <v>718</v>
+      </c>
+      <c r="BX15" s="10">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>14</v>
       </c>
@@ -4250,11 +6500,45 @@
       <c r="BA16" t="s">
         <v>362</v>
       </c>
-      <c r="BB16" s="4">
+      <c r="BB16" s="8">
+        <v>1</v>
+      </c>
+      <c r="BC16" s="10"/>
+      <c r="BD16" s="10"/>
+      <c r="BE16" s="10"/>
+      <c r="BF16" s="10"/>
+      <c r="BG16" s="10"/>
+      <c r="BH16" s="10"/>
+      <c r="BI16" s="10"/>
+      <c r="BJ16" s="10"/>
+      <c r="BK16" s="10"/>
+      <c r="BL16" s="10"/>
+      <c r="BM16" s="10"/>
+      <c r="BN16" s="10"/>
+      <c r="BO16" s="9" t="s">
+        <v>719</v>
+      </c>
+      <c r="BP16" s="10">
+        <v>1</v>
+      </c>
+      <c r="BQ16" s="10"/>
+      <c r="BR16" s="10"/>
+      <c r="BS16" s="10"/>
+      <c r="BT16" s="10"/>
+      <c r="BU16" s="9" t="s">
+        <v>720</v>
+      </c>
+      <c r="BV16" s="10">
+        <v>1</v>
+      </c>
+      <c r="BW16" s="10" t="s">
+        <v>721</v>
+      </c>
+      <c r="BX16" s="10">
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>15</v>
       </c>
@@ -4351,11 +6635,41 @@
       <c r="BA17" t="s">
         <v>363</v>
       </c>
-      <c r="BB17" s="4">
+      <c r="BB17" s="8">
+        <v>1</v>
+      </c>
+      <c r="BC17" s="10"/>
+      <c r="BD17" s="10"/>
+      <c r="BE17" s="10"/>
+      <c r="BF17" s="10"/>
+      <c r="BG17" s="10"/>
+      <c r="BH17" s="10"/>
+      <c r="BI17" s="10"/>
+      <c r="BJ17" s="10"/>
+      <c r="BK17" s="10"/>
+      <c r="BL17" s="10"/>
+      <c r="BM17" s="10"/>
+      <c r="BN17" s="10"/>
+      <c r="BO17" s="10"/>
+      <c r="BP17" s="10"/>
+      <c r="BQ17" s="10"/>
+      <c r="BR17" s="10"/>
+      <c r="BS17" s="10"/>
+      <c r="BT17" s="10"/>
+      <c r="BU17" s="9" t="s">
+        <v>722</v>
+      </c>
+      <c r="BV17" s="10">
+        <v>1</v>
+      </c>
+      <c r="BW17" s="10" t="s">
+        <v>723</v>
+      </c>
+      <c r="BX17" s="10">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>16</v>
       </c>
@@ -4446,11 +6760,41 @@
       <c r="BA18" t="s">
         <v>364</v>
       </c>
-      <c r="BB18" s="4">
+      <c r="BB18" s="8">
+        <v>1</v>
+      </c>
+      <c r="BC18" s="10"/>
+      <c r="BD18" s="10"/>
+      <c r="BE18" s="10"/>
+      <c r="BF18" s="10"/>
+      <c r="BG18" s="10"/>
+      <c r="BH18" s="10"/>
+      <c r="BI18" s="10"/>
+      <c r="BJ18" s="10"/>
+      <c r="BK18" s="10"/>
+      <c r="BL18" s="10"/>
+      <c r="BM18" s="10"/>
+      <c r="BN18" s="10"/>
+      <c r="BO18" s="10"/>
+      <c r="BP18" s="10"/>
+      <c r="BQ18" s="10"/>
+      <c r="BR18" s="10"/>
+      <c r="BS18" s="10"/>
+      <c r="BT18" s="10"/>
+      <c r="BU18" s="9" t="s">
+        <v>724</v>
+      </c>
+      <c r="BV18" s="10">
+        <v>1</v>
+      </c>
+      <c r="BW18" s="10" t="s">
+        <v>725</v>
+      </c>
+      <c r="BX18" s="10">
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>18</v>
       </c>
@@ -4541,11 +6885,41 @@
       <c r="BA19" t="s">
         <v>365</v>
       </c>
-      <c r="BB19" s="4">
+      <c r="BB19" s="8">
+        <v>1</v>
+      </c>
+      <c r="BC19" s="10"/>
+      <c r="BD19" s="10"/>
+      <c r="BE19" s="10"/>
+      <c r="BF19" s="10"/>
+      <c r="BG19" s="10"/>
+      <c r="BH19" s="10"/>
+      <c r="BI19" s="10"/>
+      <c r="BJ19" s="10"/>
+      <c r="BK19" s="10"/>
+      <c r="BL19" s="10"/>
+      <c r="BM19" s="10"/>
+      <c r="BN19" s="10"/>
+      <c r="BO19" s="10"/>
+      <c r="BP19" s="10"/>
+      <c r="BQ19" s="10"/>
+      <c r="BR19" s="10"/>
+      <c r="BS19" s="10"/>
+      <c r="BT19" s="10"/>
+      <c r="BU19" s="9" t="s">
+        <v>726</v>
+      </c>
+      <c r="BV19" s="10">
+        <v>1</v>
+      </c>
+      <c r="BW19" s="10" t="s">
+        <v>727</v>
+      </c>
+      <c r="BX19" s="10">
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>19</v>
       </c>
@@ -4630,11 +7004,41 @@
       <c r="BA20" t="s">
         <v>366</v>
       </c>
-      <c r="BB20" s="4">
+      <c r="BB20" s="8">
+        <v>1</v>
+      </c>
+      <c r="BC20" s="10"/>
+      <c r="BD20" s="10"/>
+      <c r="BE20" s="10"/>
+      <c r="BF20" s="10"/>
+      <c r="BG20" s="10"/>
+      <c r="BH20" s="10"/>
+      <c r="BI20" s="10"/>
+      <c r="BJ20" s="10"/>
+      <c r="BK20" s="10"/>
+      <c r="BL20" s="10"/>
+      <c r="BM20" s="10"/>
+      <c r="BN20" s="10"/>
+      <c r="BO20" s="10"/>
+      <c r="BP20" s="10"/>
+      <c r="BQ20" s="10"/>
+      <c r="BR20" s="10"/>
+      <c r="BS20" s="10"/>
+      <c r="BT20" s="10"/>
+      <c r="BU20" s="9" t="s">
+        <v>728</v>
+      </c>
+      <c r="BV20" s="10">
+        <v>1</v>
+      </c>
+      <c r="BW20" s="10" t="s">
+        <v>729</v>
+      </c>
+      <c r="BX20" s="10">
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>20</v>
       </c>
@@ -4719,11 +7123,41 @@
       <c r="BA21" t="s">
         <v>367</v>
       </c>
-      <c r="BB21" s="4">
+      <c r="BB21" s="8">
+        <v>1</v>
+      </c>
+      <c r="BC21" s="10"/>
+      <c r="BD21" s="10"/>
+      <c r="BE21" s="10"/>
+      <c r="BF21" s="10"/>
+      <c r="BG21" s="10"/>
+      <c r="BH21" s="10"/>
+      <c r="BI21" s="10"/>
+      <c r="BJ21" s="10"/>
+      <c r="BK21" s="10"/>
+      <c r="BL21" s="10"/>
+      <c r="BM21" s="10"/>
+      <c r="BN21" s="10"/>
+      <c r="BO21" s="10"/>
+      <c r="BP21" s="10"/>
+      <c r="BQ21" s="10"/>
+      <c r="BR21" s="10"/>
+      <c r="BS21" s="10"/>
+      <c r="BT21" s="10"/>
+      <c r="BU21" s="9" t="s">
+        <v>730</v>
+      </c>
+      <c r="BV21" s="10">
+        <v>1</v>
+      </c>
+      <c r="BW21" s="10" t="s">
+        <v>731</v>
+      </c>
+      <c r="BX21" s="10">
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>21</v>
       </c>
@@ -4802,11 +7236,37 @@
       <c r="BA22" t="s">
         <v>375</v>
       </c>
-      <c r="BB22" s="4">
+      <c r="BB22" s="8">
+        <v>1</v>
+      </c>
+      <c r="BC22" s="10"/>
+      <c r="BD22" s="10"/>
+      <c r="BE22" s="10"/>
+      <c r="BF22" s="10"/>
+      <c r="BG22" s="10"/>
+      <c r="BH22" s="10"/>
+      <c r="BI22" s="10"/>
+      <c r="BJ22" s="10"/>
+      <c r="BK22" s="10"/>
+      <c r="BL22" s="10"/>
+      <c r="BM22" s="10"/>
+      <c r="BN22" s="10"/>
+      <c r="BO22" s="10"/>
+      <c r="BP22" s="10"/>
+      <c r="BQ22" s="10"/>
+      <c r="BR22" s="10"/>
+      <c r="BS22" s="10"/>
+      <c r="BT22" s="10"/>
+      <c r="BU22" s="10"/>
+      <c r="BV22" s="10"/>
+      <c r="BW22" s="10" t="s">
+        <v>732</v>
+      </c>
+      <c r="BX22" s="10">
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>553</v>
       </c>
@@ -4885,11 +7345,37 @@
       <c r="BA23" t="s">
         <v>368</v>
       </c>
-      <c r="BB23" s="4">
+      <c r="BB23" s="8">
+        <v>1</v>
+      </c>
+      <c r="BC23" s="10"/>
+      <c r="BD23" s="10"/>
+      <c r="BE23" s="10"/>
+      <c r="BF23" s="10"/>
+      <c r="BG23" s="10"/>
+      <c r="BH23" s="10"/>
+      <c r="BI23" s="10"/>
+      <c r="BJ23" s="10"/>
+      <c r="BK23" s="10"/>
+      <c r="BL23" s="10"/>
+      <c r="BM23" s="10"/>
+      <c r="BN23" s="10"/>
+      <c r="BO23" s="10"/>
+      <c r="BP23" s="10"/>
+      <c r="BQ23" s="10"/>
+      <c r="BR23" s="10"/>
+      <c r="BS23" s="10"/>
+      <c r="BT23" s="10"/>
+      <c r="BU23" s="10"/>
+      <c r="BV23" s="10"/>
+      <c r="BW23" s="10" t="s">
+        <v>733</v>
+      </c>
+      <c r="BX23" s="10">
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>22</v>
       </c>
@@ -4961,11 +7447,37 @@
       <c r="BA24" t="s">
         <v>369</v>
       </c>
-      <c r="BB24" s="4">
+      <c r="BB24" s="8">
+        <v>1</v>
+      </c>
+      <c r="BC24" s="10"/>
+      <c r="BD24" s="10"/>
+      <c r="BE24" s="10"/>
+      <c r="BF24" s="10"/>
+      <c r="BG24" s="10"/>
+      <c r="BH24" s="10"/>
+      <c r="BI24" s="10"/>
+      <c r="BJ24" s="10"/>
+      <c r="BK24" s="10"/>
+      <c r="BL24" s="10"/>
+      <c r="BM24" s="10"/>
+      <c r="BN24" s="10"/>
+      <c r="BO24" s="10"/>
+      <c r="BP24" s="10"/>
+      <c r="BQ24" s="10"/>
+      <c r="BR24" s="10"/>
+      <c r="BS24" s="10"/>
+      <c r="BT24" s="10"/>
+      <c r="BU24" s="10"/>
+      <c r="BV24" s="10"/>
+      <c r="BW24" s="10" t="s">
+        <v>734</v>
+      </c>
+      <c r="BX24" s="10">
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>23</v>
       </c>
@@ -5037,11 +7549,37 @@
       <c r="BA25" t="s">
         <v>370</v>
       </c>
-      <c r="BB25" s="4">
+      <c r="BB25" s="8">
+        <v>1</v>
+      </c>
+      <c r="BC25" s="10"/>
+      <c r="BD25" s="10"/>
+      <c r="BE25" s="10"/>
+      <c r="BF25" s="10"/>
+      <c r="BG25" s="10"/>
+      <c r="BH25" s="10"/>
+      <c r="BI25" s="10"/>
+      <c r="BJ25" s="10"/>
+      <c r="BK25" s="10"/>
+      <c r="BL25" s="10"/>
+      <c r="BM25" s="10"/>
+      <c r="BN25" s="10"/>
+      <c r="BO25" s="10"/>
+      <c r="BP25" s="10"/>
+      <c r="BQ25" s="10"/>
+      <c r="BR25" s="10"/>
+      <c r="BS25" s="10"/>
+      <c r="BT25" s="10"/>
+      <c r="BU25" s="10"/>
+      <c r="BV25" s="10"/>
+      <c r="BW25" s="10" t="s">
+        <v>735</v>
+      </c>
+      <c r="BX25" s="10">
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>24</v>
       </c>
@@ -5109,11 +7647,37 @@
       <c r="BA26" t="s">
         <v>371</v>
       </c>
-      <c r="BB26" s="4">
+      <c r="BB26" s="8">
+        <v>1</v>
+      </c>
+      <c r="BC26" s="10"/>
+      <c r="BD26" s="10"/>
+      <c r="BE26" s="10"/>
+      <c r="BF26" s="10"/>
+      <c r="BG26" s="10"/>
+      <c r="BH26" s="10"/>
+      <c r="BI26" s="10"/>
+      <c r="BJ26" s="10"/>
+      <c r="BK26" s="10"/>
+      <c r="BL26" s="10"/>
+      <c r="BM26" s="10"/>
+      <c r="BN26" s="10"/>
+      <c r="BO26" s="10"/>
+      <c r="BP26" s="10"/>
+      <c r="BQ26" s="10"/>
+      <c r="BR26" s="10"/>
+      <c r="BS26" s="10"/>
+      <c r="BT26" s="10"/>
+      <c r="BU26" s="10"/>
+      <c r="BV26" s="10"/>
+      <c r="BW26" s="10" t="s">
+        <v>736</v>
+      </c>
+      <c r="BX26" s="10">
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>525</v>
       </c>
@@ -5171,11 +7735,37 @@
       <c r="BA27" t="s">
         <v>372</v>
       </c>
-      <c r="BB27" s="4">
+      <c r="BB27" s="8">
+        <v>1</v>
+      </c>
+      <c r="BC27" s="10"/>
+      <c r="BD27" s="10"/>
+      <c r="BE27" s="10"/>
+      <c r="BF27" s="10"/>
+      <c r="BG27" s="10"/>
+      <c r="BH27" s="10"/>
+      <c r="BI27" s="10"/>
+      <c r="BJ27" s="10"/>
+      <c r="BK27" s="10"/>
+      <c r="BL27" s="10"/>
+      <c r="BM27" s="10"/>
+      <c r="BN27" s="10"/>
+      <c r="BO27" s="10"/>
+      <c r="BP27" s="10"/>
+      <c r="BQ27" s="10"/>
+      <c r="BR27" s="10"/>
+      <c r="BS27" s="10"/>
+      <c r="BT27" s="10"/>
+      <c r="BU27" s="10"/>
+      <c r="BV27" s="10"/>
+      <c r="BW27" s="10" t="s">
+        <v>737</v>
+      </c>
+      <c r="BX27" s="10">
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>526</v>
       </c>
@@ -5231,11 +7821,37 @@
       <c r="BA28" t="s">
         <v>373</v>
       </c>
-      <c r="BB28" s="4">
+      <c r="BB28" s="8">
+        <v>1</v>
+      </c>
+      <c r="BC28" s="10"/>
+      <c r="BD28" s="10"/>
+      <c r="BE28" s="10"/>
+      <c r="BF28" s="10"/>
+      <c r="BG28" s="10"/>
+      <c r="BH28" s="10"/>
+      <c r="BI28" s="10"/>
+      <c r="BJ28" s="10"/>
+      <c r="BK28" s="10"/>
+      <c r="BL28" s="10"/>
+      <c r="BM28" s="10"/>
+      <c r="BN28" s="10"/>
+      <c r="BO28" s="10"/>
+      <c r="BP28" s="10"/>
+      <c r="BQ28" s="10"/>
+      <c r="BR28" s="10"/>
+      <c r="BS28" s="10"/>
+      <c r="BT28" s="10"/>
+      <c r="BU28" s="10"/>
+      <c r="BV28" s="10"/>
+      <c r="BW28" s="10" t="s">
+        <v>738</v>
+      </c>
+      <c r="BX28" s="10">
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>527</v>
       </c>
@@ -5285,11 +7901,37 @@
       <c r="BA29" t="s">
         <v>374</v>
       </c>
-      <c r="BB29" s="4">
+      <c r="BB29" s="8">
+        <v>1</v>
+      </c>
+      <c r="BC29" s="10"/>
+      <c r="BD29" s="10"/>
+      <c r="BE29" s="10"/>
+      <c r="BF29" s="10"/>
+      <c r="BG29" s="10"/>
+      <c r="BH29" s="10"/>
+      <c r="BI29" s="10"/>
+      <c r="BJ29" s="10"/>
+      <c r="BK29" s="10"/>
+      <c r="BL29" s="10"/>
+      <c r="BM29" s="10"/>
+      <c r="BN29" s="10"/>
+      <c r="BO29" s="10"/>
+      <c r="BP29" s="10"/>
+      <c r="BQ29" s="10"/>
+      <c r="BR29" s="10"/>
+      <c r="BS29" s="10"/>
+      <c r="BT29" s="10"/>
+      <c r="BU29" s="10"/>
+      <c r="BV29" s="10"/>
+      <c r="BW29" s="10" t="s">
+        <v>739</v>
+      </c>
+      <c r="BX29" s="10">
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>528</v>
       </c>
@@ -5336,8 +7978,29 @@
       <c r="AV30" s="4">
         <v>1</v>
       </c>
+      <c r="BC30" s="2"/>
+      <c r="BD30" s="2"/>
+      <c r="BE30" s="2"/>
+      <c r="BF30" s="2"/>
+      <c r="BG30" s="2"/>
+      <c r="BH30" s="2"/>
+      <c r="BI30" s="2"/>
+      <c r="BJ30" s="2"/>
+      <c r="BK30" s="2"/>
+      <c r="BL30" s="2"/>
+      <c r="BM30" s="2"/>
+      <c r="BN30" s="2"/>
+      <c r="BO30" s="2"/>
+      <c r="BP30" s="2"/>
+      <c r="BQ30" s="2"/>
+      <c r="BR30" s="2"/>
+      <c r="BS30" s="2"/>
+      <c r="BT30" s="2"/>
+      <c r="BU30" s="2"/>
+      <c r="BV30" s="2"/>
+      <c r="BW30" s="2"/>
     </row>
-    <row r="31" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>529</v>
       </c>
@@ -5378,8 +8041,29 @@
       <c r="AT31" s="4">
         <v>1</v>
       </c>
+      <c r="BC31" s="2"/>
+      <c r="BD31" s="2"/>
+      <c r="BE31" s="2"/>
+      <c r="BF31" s="2"/>
+      <c r="BG31" s="2"/>
+      <c r="BH31" s="2"/>
+      <c r="BI31" s="2"/>
+      <c r="BJ31" s="2"/>
+      <c r="BK31" s="2"/>
+      <c r="BL31" s="2"/>
+      <c r="BM31" s="2"/>
+      <c r="BN31" s="2"/>
+      <c r="BO31" s="2"/>
+      <c r="BP31" s="2"/>
+      <c r="BQ31" s="2"/>
+      <c r="BR31" s="2"/>
+      <c r="BS31" s="2"/>
+      <c r="BT31" s="2"/>
+      <c r="BU31" s="2"/>
+      <c r="BV31" s="2"/>
+      <c r="BW31" s="2"/>
     </row>
-    <row r="32" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>530</v>
       </c>
@@ -6341,5 +9025,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>